<commit_message>
CSV support + 900k test
</commit_message>
<xml_diff>
--- a/uploads/processed_data.xlsx
+++ b/uploads/processed_data.xlsx
@@ -17,13 +17,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
+    <t>Account Number</t>
+  </si>
+  <si>
     <t>Client Code</t>
   </si>
   <si>
     <t>Customer ID</t>
-  </si>
-  <si>
-    <t>Account Number</t>
   </si>
   <si>
     <t>1234</t>
@@ -360,10 +360,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -371,10 +371,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>